<commit_message>
Added few examples to example_column in the file
</commit_message>
<xml_diff>
--- a/public/documentation/aact_beta_views.xlsx
+++ b/public/documentation/aact_beta_views.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abykova/Projects/aact-admin/public/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD43FABD-1DAE-BB4B-94E5-FA20E459C68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6A9F80-8783-1B42-926F-2EF70E04A01D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>db schema</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>nct_id &amp; names: string containing comma delimited list of condtions</t>
-  </si>
-  <si>
-    <t>select * from all_conditions where nct_id = '';</t>
   </si>
   <si>
     <t>all_countries</t>
@@ -224,12 +221,25 @@
   <si>
     <t>ctgov_beta</t>
   </si>
+  <si>
+    <t>NCT00000919 | Italy|Puerto Rico|United States</t>
+  </si>
+  <si>
+    <t>select * from all_conditions where nct_id = '';
+NCT00000146 | Multiple Sclerosis|Neuritis|Optic Neuritis</t>
+  </si>
+  <si>
+    <t>NCT00000403 | University of Arizona Arthritis Center|University of Pittsburgh Medical Center|Arthritis Research Center Foundation|Indiana University Medical Center|Northwestern University Medical Center|University of Alabama at Birmingham</t>
+  </si>
+  <si>
+    <t>NCT00000208 | Drug use|Opiate craving|Withdrawal symptoms</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -255,6 +265,12 @@
       <sz val="12"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -276,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -295,6 +311,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -572,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -583,7 +602,7 @@
     <col min="3" max="3" width="46.83203125" customWidth="1"/>
     <col min="4" max="4" width="32.5" customWidth="1"/>
     <col min="5" max="5" width="34.83203125" customWidth="1"/>
-    <col min="6" max="6" width="49.33203125" customWidth="1"/>
+    <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
     <col min="7" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -629,7 +648,7 @@
     </row>
     <row r="2" spans="1:26" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
@@ -643,8 +662,8 @@
       <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
+      <c r="F2" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -669,21 +688,23 @@
     </row>
     <row r="3" spans="1:26" ht="51" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3"/>
       <c r="G3" s="5"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -707,19 +728,21 @@
     </row>
     <row r="4" spans="1:26" ht="51" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>17</v>
+      <c r="F4" s="8" t="s">
+        <v>68</v>
       </c>
-      <c r="F4" s="3"/>
       <c r="G4" s="5"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -741,23 +764,25 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" ht="51" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" ht="85" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>21</v>
+      <c r="F5" s="4" t="s">
+        <v>67</v>
       </c>
-      <c r="F5" s="3"/>
       <c r="G5" s="5"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -781,19 +806,19 @@
     </row>
     <row r="6" spans="1:26" ht="34" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -819,19 +844,19 @@
     </row>
     <row r="7" spans="1:26" ht="34" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -857,19 +882,19 @@
     </row>
     <row r="8" spans="1:26" ht="34" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -895,19 +920,19 @@
     </row>
     <row r="9" spans="1:26" ht="51" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="5"/>
@@ -933,19 +958,19 @@
     </row>
     <row r="10" spans="1:26" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="5"/>
@@ -971,19 +996,19 @@
     </row>
     <row r="11" spans="1:26" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="5"/>
@@ -1009,19 +1034,19 @@
     </row>
     <row r="12" spans="1:26" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="5"/>
@@ -1047,19 +1072,19 @@
     </row>
     <row r="13" spans="1:26" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="5"/>
@@ -1085,19 +1110,19 @@
     </row>
     <row r="14" spans="1:26" ht="34" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="5"/>
@@ -1123,19 +1148,19 @@
     </row>
     <row r="15" spans="1:26" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1161,19 +1186,19 @@
     </row>
     <row r="16" spans="1:26" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>

</xml_diff>

<commit_message>
Added examples to the file
</commit_message>
<xml_diff>
--- a/public/documentation/aact_beta_views.xlsx
+++ b/public/documentation/aact_beta_views.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abykova/Projects/aact-admin/public/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6A9F80-8783-1B42-926F-2EF70E04A01D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7BC96D-00A6-D948-80A5-616DE4B27A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AACT Tables and Columns" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
   <si>
     <t>db schema</t>
   </si>
@@ -225,21 +225,53 @@
     <t>NCT00000919 | Italy|Puerto Rico|United States</t>
   </si>
   <si>
-    <t>select * from all_conditions where nct_id = '';
-NCT00000146 | Multiple Sclerosis|Neuritis|Optic Neuritis</t>
-  </si>
-  <si>
     <t>NCT00000403 | University of Arizona Arthritis Center|University of Pittsburgh Medical Center|Arthritis Research Center Foundation|Indiana University Medical Center|Northwestern University Medical Center|University of Alabama at Birmingham</t>
   </si>
   <si>
     <t>NCT00000208 | Drug use|Opiate craving|Withdrawal symptoms</t>
+  </si>
+  <si>
+    <t>NCT00000146 | Multiple Sclerosis|Neuritis|Optic Neuritis</t>
+  </si>
+  <si>
+    <t>NCT00002569 | Active Comparator|Experimental</t>
+  </si>
+  <si>
+    <t>NCT03803644 | CC-92480-CP-001|U1111-1224-6768</t>
+  </si>
+  <si>
+    <t>NCT03802422 | Vitamin B Complex|Hydroxocobalamin|Vitamin B 12|Vitamins</t>
+  </si>
+  <si>
+    <t>NCT03802994 | Drug|Biological|Other</t>
+  </si>
+  <si>
+    <t>NCT03801915 | Pancreas and Liver Resections|Recurrence Free Survival|Well Tolerated Agent</t>
+  </si>
+  <si>
+    <t>NCT03802162 | AUCt of D324|AUCt of D797|Cmax of D324|Cmax of D797</t>
+  </si>
+  <si>
+    <t>NCT03803397 | Overall Survival|Progression-Free Survival|Tumor Response</t>
+  </si>
+  <si>
+    <t>NCT03803254 | Guangzhou No.12 People's Hospital|Kaiping Central Hospital|Sun Yat-sen University</t>
+  </si>
+  <si>
+    <t>NCT03802877 | Alberta|Manitoba|Ontario|Quebec</t>
+  </si>
+  <si>
+    <t>Refer to the covid_19 spreadsheets on the downloads page</t>
+  </si>
+  <si>
+    <t>1|NCT04559945|covid-19|Wed, 13 Oct 2021 13:19:25 EDT -04:00|Wed, 13 Oct 2021 13:19:25 EDT -04:00|covid-19|2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -271,6 +303,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -292,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -315,6 +353,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,14 +636,14 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="46.83203125" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.5" customWidth="1"/>
     <col min="5" max="5" width="34.83203125" customWidth="1"/>
     <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
@@ -663,7 +707,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -702,7 +746,7 @@
       <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G3" s="5"/>
@@ -741,7 +785,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="3"/>
@@ -781,7 +825,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="3"/>
@@ -820,7 +864,9 @@
       <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -858,7 +904,9 @@
       <c r="E7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -896,7 +944,9 @@
       <c r="E8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -934,7 +984,9 @@
       <c r="E9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -956,7 +1008,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" ht="51" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>64</v>
       </c>
@@ -972,7 +1024,9 @@
       <c r="E10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1010,7 +1064,9 @@
       <c r="E11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="G11" s="5"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -1048,7 +1104,9 @@
       <c r="E12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -1086,7 +1144,9 @@
       <c r="E13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="G13" s="5"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -1124,7 +1184,9 @@
       <c r="E14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="G14" s="5"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -1162,7 +1224,9 @@
       <c r="E15" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -1200,7 +1264,9 @@
       <c r="E16" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="9" t="s">
+        <v>78</v>
+      </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>

</xml_diff>

<commit_message>
Added description to all_design_outcomes
</commit_message>
<xml_diff>
--- a/public/documentation/aact_beta_views.xlsx
+++ b/public/documentation/aact_beta_views.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abykova/Projects/aact-admin/public/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7BC96D-00A6-D948-80A5-616DE4B27A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4245497-B149-D04B-8B6A-78398DF36A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t>db schema</t>
   </si>
@@ -266,12 +266,15 @@
   <si>
     <t>1|NCT04559945|covid-19|Wed, 13 Oct 2021 13:19:25 EDT -04:00|Wed, 13 Oct 2021 13:19:25 EDT -04:00|covid-19|2</t>
   </si>
+  <si>
+    <t>concatenated list of the all design_outcome measures associated with a study</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -282,20 +285,24 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -306,6 +313,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -330,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -358,6 +371,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -636,7 +652,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -777,7 +793,9 @@
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="11" t="s">
+        <v>80</v>
+      </c>
       <c r="D4" s="4" t="s">
         <v>15</v>
       </c>

</xml_diff>